<commit_message>
Anzahl der Oszillationen werden über das settings file festgelegt.
</commit_message>
<xml_diff>
--- a/Einstellungen/EinstellungenSimple.xlsx
+++ b/Einstellungen/EinstellungenSimple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20730" windowHeight="10320" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20730" windowHeight="10320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Amplitude</t>
   </si>
@@ -40,15 +40,6 @@
     <t>Fokus</t>
   </si>
   <si>
-    <t>Länge</t>
-  </si>
-  <si>
-    <t>Breite</t>
-  </si>
-  <si>
-    <t>Tiefe</t>
-  </si>
-  <si>
     <t>Diskretisierung</t>
   </si>
   <si>
@@ -92,6 +83,27 @@
   </si>
   <si>
     <t>Dz</t>
+  </si>
+  <si>
+    <t>Anzahl der Ozillationen</t>
+  </si>
+  <si>
+    <t>Xstart</t>
+  </si>
+  <si>
+    <t>Ystart</t>
+  </si>
+  <si>
+    <t>Zstart</t>
+  </si>
+  <si>
+    <t>Xend</t>
+  </si>
+  <si>
+    <t>Zend</t>
+  </si>
+  <si>
+    <t>Yend</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,46 +506,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>4.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="B2" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>5.0000000000000002E-5</v>
@@ -544,16 +563,25 @@
       <c r="F2" s="2">
         <v>3.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>4.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="B3" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <v>5.0000000000000002E-5</v>
@@ -563,6 +591,15 @@
       </c>
       <c r="F3" s="2">
         <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2E-3</v>
       </c>
     </row>
   </sheetData>
@@ -593,28 +630,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -690,10 +727,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -719,43 +756,54 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1E-3</v>
       </c>
       <c r="B2" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1E-3</v>
       </c>
       <c r="B3" s="3">
         <v>40</v>
       </c>
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Änderungen nach DA Übergabe III
</commit_message>
<xml_diff>
--- a/Einstellungen/EinstellungenSimple.xlsx
+++ b/Einstellungen/EinstellungenSimple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20730" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="17700" windowHeight="8025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
     <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,8 +109,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,7 +162,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,16 +439,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
@@ -476,28 +476,18 @@
         <v>1.6E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>300</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -505,17 +495,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -544,63 +536,45 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>5.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E2" s="2">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E2" s="2">
-        <v>4.0000000000000003E-5</v>
-      </c>
       <c r="F2" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="G2" s="2">
-        <v>4.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H2" s="2">
         <v>2E-3</v>
       </c>
       <c r="I2" s="2">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2E-3</v>
-      </c>
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -609,14 +583,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -628,7 +602,7 @@
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -654,15 +628,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3">
-        <v>33.630000000000003</v>
+        <v>30.5</v>
       </c>
       <c r="B2" s="3">
-        <v>7033</v>
+        <v>7035</v>
       </c>
       <c r="C2" s="3">
-        <v>711.4</v>
+        <v>492</v>
       </c>
       <c r="D2" s="3">
         <v>0.25</v>
@@ -671,7 +645,7 @@
         <v>275000</v>
       </c>
       <c r="F2" s="3">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="G2" s="3">
         <v>3133</v>
@@ -680,31 +654,15 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>33.630000000000003</v>
-      </c>
-      <c r="B3" s="3">
-        <v>7033</v>
-      </c>
-      <c r="C3" s="3">
-        <v>711.4</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="3">
-        <v>275000</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1796</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3133</v>
-      </c>
-      <c r="H3" s="3">
-        <v>300</v>
-      </c>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -712,20 +670,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -733,7 +691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="5">
         <v>1.0640000000000001E-6</v>
       </c>
@@ -741,13 +699,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1.0640000000000001E-6</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2.5000000000000001E-5</v>
-      </c>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -755,21 +709,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -780,27 +734,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1E-3</v>
       </c>
       <c r="B2" s="3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>40</v>
-      </c>
-      <c r="C3" s="3">
-        <v>10</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Temperaturfelder werden auf Verdampfungstemperatur gedeckelt --> Werte darüber sind nicht sinnvoll und entstehen nur durch Superposition.
</commit_message>
<xml_diff>
--- a/Einstellungen/EinstellungenSimple.xlsx
+++ b/Einstellungen/EinstellungenSimple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="17700" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="17700" windowHeight="8025" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -742,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>